<commit_message>
uploaded charts used in final presentation
</commit_message>
<xml_diff>
--- a/Final Report/replication_viz.xlsx
+++ b/Final Report/replication_viz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Downloads/GitHub/COMP8240_Project_J/Final Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A2DC66CD-F8F2-DF45-A2C1-65215723F7F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E271C0F-70E7-7045-9670-CDF22819E153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="label" sheetId="1" r:id="rId1"/>
@@ -954,7 +954,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -2203,7 +2203,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Replication Results Accuracy</a:t>
+              <a:t>Replication Results on Original and New Data</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2332,16 +2332,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Text Only</c:v>
+                  <c:v>Multimodal-Attention</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Multimodal</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Audio Only</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Multimodal</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Multimodal-Attention</c:v>
+                  <c:v>Text Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2353,16 +2353,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.308</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36299999999999999</c:v>
+                  <c:v>0.34899999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35</c:v>
+                  <c:v>0.30599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2461,16 +2461,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Text Only</c:v>
+                  <c:v>Multimodal-Attention</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Multimodal</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Audio Only</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Multimodal</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Multimodal-Attention</c:v>
+                  <c:v>Text Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2482,16 +2482,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.32700000000000001</c:v>
+                  <c:v>0.2389</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.23499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27300000000000002</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2389</c:v>
+                  <c:v>0.32700000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2590,16 +2590,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Text Only</c:v>
+                  <c:v>Multimodal-Attention</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Multimodal</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Audio Only</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Multimodal</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Multimodal-Attention</c:v>
+                  <c:v>Text Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2611,16 +2611,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.628</c:v>
+                  <c:v>0.48499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.55700000000000005</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.71</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48499999999999999</c:v>
+                  <c:v>0.628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2719,16 +2719,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Text Only</c:v>
+                  <c:v>Multimodal-Attention</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Multimodal</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Audio Only</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Multimodal</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Multimodal-Attention</c:v>
+                  <c:v>Text Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2740,16 +2740,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.63500000000000001</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.71799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.54600000000000004</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.71799999999999997</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69</c:v>
+                  <c:v>0.63500000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5452,16 +5452,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z285"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:U285"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5511,22 +5511,22 @@
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="L3" s="2">
-        <v>0.63500000000000001</v>
+        <v>0.69</v>
       </c>
       <c r="M3" s="2">
-        <v>0.628</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="N3" s="2">
-        <v>0.32700000000000001</v>
+        <v>0.2389</v>
       </c>
       <c r="O3" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5544,22 +5544,22 @@
         <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L4" s="2">
-        <v>0.54600000000000004</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="M4" s="2">
-        <v>0.55700000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="N4" s="2">
-        <v>0.23499999999999999</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="O4" s="2">
-        <v>0.36299999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0.34899999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -5577,22 +5577,22 @@
         <v>52</v>
       </c>
       <c r="K5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L5" s="2">
-        <v>0.71799999999999997</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="M5" s="2">
-        <v>0.71</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="N5" s="2">
-        <v>0.27300000000000002</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="O5" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5610,27 +5610,27 @@
         <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="L6" s="2">
-        <v>0.69</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="M6" s="2">
-        <v>0.48499999999999999</v>
+        <v>0.628</v>
       </c>
       <c r="N6" s="2">
-        <v>0.2389</v>
+        <v>0.32700000000000001</v>
       </c>
       <c r="O6" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -5647,13 +5647,13 @@
         <f>COUNTIF(C:C,E7)</f>
         <v>22</v>
       </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -5663,13 +5663,13 @@
       <c r="C8" t="s">
         <v>290</v>
       </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -5685,13 +5685,13 @@
       <c r="F9" t="s">
         <v>295</v>
       </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -5707,13 +5707,13 @@
       <c r="F10">
         <v>400</v>
       </c>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -8772,7 +8772,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C285"/>
+  <autoFilter ref="A2:C285" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:F7">
     <sortCondition descending="1" ref="F3:F7"/>
   </sortState>

</xml_diff>